<commit_message>
Sprint3-Added report properties file
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/DsAlgo_TestData.xlsx
+++ b/src/test/resources/TestData/DsAlgo_TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rinuh\eclipse-workspace\DsAlgo_CodeCrackers\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77FB18F4-DFB1-4DD0-B9A2-11CE8DC28E6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0816FCB5-1D74-4708-ACC6-F930B8481840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{768FEF77-440B-4D31-8900-E6875843D333}"/>
   </bookViews>
@@ -137,7 +137,7 @@
     <t>code@123</t>
   </si>
   <si>
-    <t>Admin@12345</t>
+    <t>Admin1@567</t>
   </si>
 </sst>
 </file>
@@ -653,8 +653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{492C72F3-3731-4F88-9CA8-7DD609FA2336}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Latest without null pointer exception
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/DsAlgo_TestData.xlsx
+++ b/src/test/resources/TestData/DsAlgo_TestData.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rinuh\eclipse-workspace\DsAlgo_CodeCrackers\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rinuh\git\DsAlgo_CodeCrackers_BDD\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0816FCB5-1D74-4708-ACC6-F930B8481840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58DF25BF-F823-4D18-8B1C-E6473C52B883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{768FEF77-440B-4D31-8900-E6875843D333}"/>
   </bookViews>
   <sheets>
-    <sheet name="Login" sheetId="2" r:id="rId1"/>
-    <sheet name="Register" sheetId="1" r:id="rId2"/>
-    <sheet name="TryEditor" sheetId="3" r:id="rId3"/>
-    <sheet name="Array" sheetId="4" r:id="rId4"/>
+    <sheet name="Login_Valid" sheetId="5" r:id="rId1"/>
+    <sheet name="Login" sheetId="2" r:id="rId2"/>
+    <sheet name="Register" sheetId="1" r:id="rId3"/>
+    <sheet name="TryEditor" sheetId="3" r:id="rId4"/>
+    <sheet name="Array" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
   <si>
     <t xml:space="preserve">USERNAME </t>
   </si>
@@ -138,6 +139,12 @@
   </si>
   <si>
     <t>Admin1@567</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
   </si>
 </sst>
 </file>
@@ -228,7 +235,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -242,6 +249,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -576,11 +584,50 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E41D17D7-B87F-4182-9263-EEBD884F05B2}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{2E5CF1F5-45E5-47B9-9545-006EEB78E47A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E670BE02-141A-4D4F-B91E-EA47695CA007}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -629,12 +676,8 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>8</v>
-      </c>
+      <c r="A6" s="4"/>
+      <c r="B6" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -642,18 +685,17 @@
     <hyperlink ref="A3" r:id="rId2" xr:uid="{D0EE70DA-EFCE-4257-A6F3-2F082177429B}"/>
     <hyperlink ref="A4" r:id="rId3" xr:uid="{9E8FCA4F-480C-4F45-9CF9-B9F0CDAD6ACD}"/>
     <hyperlink ref="B5" r:id="rId4" xr:uid="{20885189-DAD3-4C32-B447-5C27B6D3FF18}"/>
-    <hyperlink ref="B6" r:id="rId5" xr:uid="{8DE479F9-9210-4BBB-AD06-CE13B246C57C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{492C72F3-3731-4F88-9CA8-7DD609FA2336}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
@@ -829,7 +871,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A173DD0-45E9-468F-AA82-A822C8564EFB}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -880,7 +922,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{737527C9-A8F1-45BF-8669-5D751FF8CFC5}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>